<commit_message>
Fix time and complete test settup
</commit_message>
<xml_diff>
--- a/MaterielTest/Inscriptions_1.xlsx
+++ b/MaterielTest/Inscriptions_1.xlsx
@@ -5,29 +5,29 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
-    <sheet name="Renseignement" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Ecolière B" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Ecolier B" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Ecolière A" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="Ecolier A" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="Espoir F" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="Espoir M" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="Junior F" sheetId="8" state="visible" r:id="rId10"/>
-    <sheet name="Junior M" sheetId="9" state="visible" r:id="rId11"/>
-    <sheet name="Elite F" sheetId="10" state="visible" r:id="rId12"/>
-    <sheet name="Elite M" sheetId="11" state="visible" r:id="rId13"/>
-    <sheet name="Vétéran F" sheetId="12" state="visible" r:id="rId14"/>
-    <sheet name="Vétéran M" sheetId="13" state="visible" r:id="rId15"/>
-    <sheet name="Open F" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="Open M" sheetId="15" state="visible" r:id="rId17"/>
-    <sheet name="Club" sheetId="16" state="hidden" r:id="rId18"/>
-    <sheet name="Genre" sheetId="17" state="hidden" r:id="rId19"/>
-    <sheet name="Ceinture" sheetId="18" state="hidden" r:id="rId20"/>
-    <sheet name="Catégories" sheetId="19" state="hidden" r:id="rId21"/>
-    <sheet name="config" sheetId="20" state="visible" r:id="rId22"/>
+    <sheet name="Renseignement" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Ecolière B" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Ecolier B" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Ecolière A" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Ecolier A" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Espoir F" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Espoir M" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Junior F" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Junior M" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Elite F" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Elite M" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Vétéran F" sheetId="12" state="hidden" r:id="rId13"/>
+    <sheet name="Vétéran M" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Open F" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Open M" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Club" sheetId="16" state="hidden" r:id="rId17"/>
+    <sheet name="Genre" sheetId="17" state="hidden" r:id="rId18"/>
+    <sheet name="Ceinture" sheetId="18" state="hidden" r:id="rId19"/>
+    <sheet name="Catégories" sheetId="19" state="hidden" r:id="rId20"/>
+    <sheet name="config" sheetId="20" state="visible" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="F13_Ecolière_B" vbProcedure="false">Catégories!$G$3:$G$11</definedName>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="147">
   <si>
     <t xml:space="preserve">Inscriptions pour les Championat Genevois </t>
   </si>
@@ -180,7 +180,7 @@
     <t xml:space="preserve">Renaud</t>
   </si>
   <si>
-    <t xml:space="preserve">-73</t>
+    <t xml:space="preserve">'-73</t>
   </si>
   <si>
     <t xml:space="preserve">Elite F</t>
@@ -189,28 +189,49 @@
     <t xml:space="preserve">Elite M</t>
   </si>
   <si>
-    <t xml:space="preserve">Giraudt</t>
+    <t xml:space="preserve">Manuel</t>
   </si>
   <si>
-    <t xml:space="preserve">Lambert</t>
+    <t xml:space="preserve">Raoul</t>
   </si>
   <si>
-    <t xml:space="preserve">Auguste</t>
+    <t xml:space="preserve">Etienne</t>
   </si>
   <si>
-    <t xml:space="preserve">Maxime</t>
+    <t xml:space="preserve">-73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">François</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul</t>
   </si>
   <si>
     <t xml:space="preserve">-81</t>
   </si>
   <si>
-    <t xml:space="preserve">Vaugrenard</t>
+    <t xml:space="preserve">René</t>
   </si>
   <si>
-    <t xml:space="preserve">José</t>
+    <t xml:space="preserve">Théo</t>
   </si>
   <si>
     <t xml:space="preserve">-90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Léo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eloi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valerain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+90</t>
   </si>
   <si>
     <t xml:space="preserve">Vétéran F (&gt;30)</t>
@@ -429,9 +450,6 @@
     <t xml:space="preserve">'-63</t>
   </si>
   <si>
-    <t xml:space="preserve">'-73</t>
-  </si>
-  <si>
     <t xml:space="preserve">-50</t>
   </si>
   <si>
@@ -451,9 +469,6 @@
   </si>
   <si>
     <t xml:space="preserve">-52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+90</t>
   </si>
   <si>
     <t xml:space="preserve">+40</t>
@@ -487,14 +502,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="167" formatCode="[$-100C]dd/mm/yyyy"/>
-    <numFmt numFmtId="168" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
+    <numFmt numFmtId="168" formatCode="@"/>
+    <numFmt numFmtId="169" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -534,12 +550,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -750,7 +760,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -819,15 +829,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -847,7 +857,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -867,6 +877,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -875,7 +897,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -887,11 +909,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -903,7 +921,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1002,9 +1020,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>702720</xdr:colOff>
+      <xdr:colOff>702000</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1018,7 +1036,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3687840" y="2378520"/>
-          <a:ext cx="2704320" cy="2704320"/>
+          <a:ext cx="2703600" cy="2703600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1033,112 +1051,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1146,8 +1058,8 @@
   </sheetPr>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1907,8 +1819,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2825,8 +2737,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2914,10 +2826,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E5" s="22" t="n">
         <v>38718</v>
@@ -2928,10 +2840,10 @@
       <c r="G5" s="23" t="n">
         <v>800004</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="32" t="b">
+      <c r="I5" s="35" t="b">
         <f aca="false">IF($E5&lt;&gt;"",AND(config!$B$1-YEAR($E5)&gt;=Catégories!$C$16,config!$B$1-YEAR($E5)&lt;Catégories!$D$16),"")</f>
         <v>0</v>
       </c>
@@ -2945,11 +2857,11 @@
       <c r="B6" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>45</v>
+      <c r="C6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="E6" s="22" t="n">
         <v>36526</v>
@@ -2960,10 +2872,10 @@
       <c r="G6" s="23" t="n">
         <v>800008</v>
       </c>
-      <c r="H6" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" s="32" t="b">
+      <c r="H6" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="35" t="b">
         <f aca="false">IF($E6&lt;&gt;"",AND(config!$B$1-YEAR($E6)&gt;=Catégories!$C$16,config!$B$1-YEAR($E6)&lt;Catégories!$D$16),"")</f>
         <v>1</v>
       </c>
@@ -2974,11 +2886,11 @@
       <c r="B7" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>47</v>
+      <c r="C7" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="E7" s="22" t="n">
         <v>36526</v>
@@ -2989,10 +2901,10 @@
       <c r="G7" s="23" t="n">
         <v>800006</v>
       </c>
-      <c r="H7" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="32" t="b">
+      <c r="H7" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="35" t="b">
         <f aca="false">IF($E7&lt;&gt;"",AND(config!$B$1-YEAR($E7)&gt;=Catégories!$C$16,config!$B$1-YEAR($E7)&lt;Catégories!$D$16),"")</f>
         <v>1</v>
       </c>
@@ -3004,10 +2916,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E8" s="22" t="n">
         <v>29221</v>
@@ -3018,10 +2930,10 @@
       <c r="G8" s="23" t="n">
         <v>800007</v>
       </c>
-      <c r="H8" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" s="32" t="b">
+      <c r="H8" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="35" t="b">
         <f aca="false">IF($E8&lt;&gt;"",AND(config!$B$1-YEAR($E8)&gt;=Catégories!$C$16,config!$B$1-YEAR($E8)&lt;Catégories!$D$16),"")</f>
         <v>1</v>
       </c>
@@ -3032,15 +2944,27 @@
       <c r="B9" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="1" t="str">
+      <c r="C9" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="22" t="n">
+        <v>36526</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="23" t="n">
+        <v>800009</v>
+      </c>
+      <c r="H9" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="35" t="b">
         <f aca="false">IF($E9&lt;&gt;"",AND(config!$B$1-YEAR($E9)&gt;=Catégories!$C$16,config!$B$1-YEAR($E9)&lt;Catégories!$D$16),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -3049,15 +2973,27 @@
       <c r="B10" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="1" t="str">
+      <c r="C10" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="22" t="n">
+        <v>36526</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="23" t="n">
+        <v>800010</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="35" t="b">
         <f aca="false">IF($E10&lt;&gt;"",AND(config!$B$1-YEAR($E10)&gt;=Catégories!$C$16,config!$B$1-YEAR($E10)&lt;Catégories!$D$16),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="J10" s="1"/>
     </row>
@@ -3071,7 +3007,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
-      <c r="H11" s="34"/>
+      <c r="H11" s="37"/>
       <c r="I11" s="1" t="str">
         <f aca="false">IF($E11&lt;&gt;"",AND(config!$B$1-YEAR($E11)&gt;=Catégories!$C$16,config!$B$1-YEAR($E11)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3089,9 +3025,9 @@
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="23"/>
-      <c r="H12" s="34"/>
+      <c r="H12" s="37"/>
       <c r="I12" s="1" t="str">
         <f aca="false">IF($E12&lt;&gt;"",AND(config!$B$1-YEAR($E12)&gt;=Catégories!$C$16,config!$B$1-YEAR($E12)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3109,9 +3045,9 @@
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="34"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="37"/>
       <c r="I13" s="1" t="str">
         <f aca="false">IF($E13&lt;&gt;"",AND(config!$B$1-YEAR($E13)&gt;=Catégories!$C$16,config!$B$1-YEAR($E13)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3129,9 +3065,9 @@
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
+      <c r="F14" s="36"/>
       <c r="G14" s="23"/>
-      <c r="H14" s="34"/>
+      <c r="H14" s="37"/>
       <c r="I14" s="1" t="str">
         <f aca="false">IF($E14&lt;&gt;"",AND(config!$B$1-YEAR($E14)&gt;=Catégories!$C$16,config!$B$1-YEAR($E14)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3149,9 +3085,9 @@
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
-      <c r="F15" s="23"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="23"/>
-      <c r="H15" s="34"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="1" t="str">
         <f aca="false">IF($E15&lt;&gt;"",AND(config!$B$1-YEAR($E15)&gt;=Catégories!$C$16,config!$B$1-YEAR($E15)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3169,9 +3105,9 @@
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
       <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
+      <c r="F16" s="36"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="34"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="1" t="str">
         <f aca="false">IF($E16&lt;&gt;"",AND(config!$B$1-YEAR($E16)&gt;=Catégories!$C$16,config!$B$1-YEAR($E16)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3191,7 +3127,7 @@
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
-      <c r="H17" s="34"/>
+      <c r="H17" s="24"/>
       <c r="I17" s="1" t="str">
         <f aca="false">IF($E17&lt;&gt;"",AND(config!$B$1-YEAR($E17)&gt;=Catégories!$C$16,config!$B$1-YEAR($E17)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3211,7 +3147,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
-      <c r="H18" s="34"/>
+      <c r="H18" s="24"/>
       <c r="I18" s="1" t="str">
         <f aca="false">IF($E18&lt;&gt;"",AND(config!$B$1-YEAR($E18)&gt;=Catégories!$C$16,config!$B$1-YEAR($E18)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3231,7 +3167,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="23"/>
       <c r="G19" s="23"/>
-      <c r="H19" s="34"/>
+      <c r="H19" s="24"/>
       <c r="I19" s="1" t="str">
         <f aca="false">IF($E19&lt;&gt;"",AND(config!$B$1-YEAR($E19)&gt;=Catégories!$C$16,config!$B$1-YEAR($E19)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3251,7 +3187,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="23"/>
       <c r="G20" s="23"/>
-      <c r="H20" s="34"/>
+      <c r="H20" s="24"/>
       <c r="I20" s="1" t="str">
         <f aca="false">IF($E20&lt;&gt;"",AND(config!$B$1-YEAR($E20)&gt;=Catégories!$C$16,config!$B$1-YEAR($E20)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3271,7 +3207,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="23"/>
       <c r="G21" s="23"/>
-      <c r="H21" s="34"/>
+      <c r="H21" s="24"/>
       <c r="I21" s="1" t="str">
         <f aca="false">IF($E21&lt;&gt;"",AND(config!$B$1-YEAR($E21)&gt;=Catégories!$C$16,config!$B$1-YEAR($E21)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3288,7 +3224,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="23"/>
       <c r="G22" s="23"/>
-      <c r="H22" s="34"/>
+      <c r="H22" s="24"/>
       <c r="I22" s="1" t="str">
         <f aca="false">IF($E22&lt;&gt;"",AND(config!$B$1-YEAR($E22)&gt;=Catégories!$C$16,config!$B$1-YEAR($E22)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3305,7 +3241,7 @@
       <c r="E23" s="22"/>
       <c r="F23" s="23"/>
       <c r="G23" s="23"/>
-      <c r="H23" s="34"/>
+      <c r="H23" s="24"/>
       <c r="I23" s="1" t="str">
         <f aca="false">IF($E23&lt;&gt;"",AND(config!$B$1-YEAR($E23)&gt;=Catégories!$C$16,config!$B$1-YEAR($E23)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3322,7 +3258,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="23"/>
       <c r="G24" s="23"/>
-      <c r="H24" s="34"/>
+      <c r="H24" s="24"/>
       <c r="I24" s="1" t="str">
         <f aca="false">IF($E24&lt;&gt;"",AND(config!$B$1-YEAR($E24)&gt;=Catégories!$C$16,config!$B$1-YEAR($E24)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3339,7 +3275,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="23"/>
       <c r="G25" s="23"/>
-      <c r="H25" s="34"/>
+      <c r="H25" s="24"/>
       <c r="I25" s="1" t="str">
         <f aca="false">IF($E25&lt;&gt;"",AND(config!$B$1-YEAR($E25)&gt;=Catégories!$C$16,config!$B$1-YEAR($E25)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3356,7 +3292,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="23"/>
       <c r="G26" s="23"/>
-      <c r="H26" s="34"/>
+      <c r="H26" s="24"/>
       <c r="I26" s="1" t="str">
         <f aca="false">IF($E26&lt;&gt;"",AND(config!$B$1-YEAR($E26)&gt;=Catégories!$C$16,config!$B$1-YEAR($E26)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3373,7 +3309,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
-      <c r="H27" s="34"/>
+      <c r="H27" s="24"/>
       <c r="I27" s="1" t="str">
         <f aca="false">IF($E27&lt;&gt;"",AND(config!$B$1-YEAR($E27)&gt;=Catégories!$C$16,config!$B$1-YEAR($E27)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3390,7 +3326,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="23"/>
       <c r="G28" s="23"/>
-      <c r="H28" s="34"/>
+      <c r="H28" s="24"/>
       <c r="I28" s="1" t="str">
         <f aca="false">IF($E28&lt;&gt;"",AND(config!$B$1-YEAR($E28)&gt;=Catégories!$C$16,config!$B$1-YEAR($E28)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3407,7 +3343,7 @@
       <c r="E29" s="22"/>
       <c r="F29" s="23"/>
       <c r="G29" s="23"/>
-      <c r="H29" s="34"/>
+      <c r="H29" s="24"/>
       <c r="I29" s="1" t="str">
         <f aca="false">IF($E29&lt;&gt;"",AND(config!$B$1-YEAR($E29)&gt;=Catégories!$C$16,config!$B$1-YEAR($E29)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3424,7 +3360,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="23"/>
       <c r="G30" s="23"/>
-      <c r="H30" s="34"/>
+      <c r="H30" s="24"/>
       <c r="I30" s="1" t="str">
         <f aca="false">IF($E30&lt;&gt;"",AND(config!$B$1-YEAR($E30)&gt;=Catégories!$C$16,config!$B$1-YEAR($E30)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3441,7 +3377,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="23"/>
       <c r="G31" s="23"/>
-      <c r="H31" s="34"/>
+      <c r="H31" s="24"/>
       <c r="I31" s="1" t="str">
         <f aca="false">IF($E31&lt;&gt;"",AND(config!$B$1-YEAR($E31)&gt;=Catégories!$C$16,config!$B$1-YEAR($E31)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3458,7 +3394,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
-      <c r="H32" s="34"/>
+      <c r="H32" s="24"/>
       <c r="I32" s="1" t="str">
         <f aca="false">IF($E32&lt;&gt;"",AND(config!$B$1-YEAR($E32)&gt;=Catégories!$C$16,config!$B$1-YEAR($E32)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3475,7 +3411,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>
-      <c r="H33" s="34"/>
+      <c r="H33" s="24"/>
       <c r="I33" s="1" t="str">
         <f aca="false">IF($E33&lt;&gt;"",AND(config!$B$1-YEAR($E33)&gt;=Catégories!$C$16,config!$B$1-YEAR($E33)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3492,7 +3428,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
-      <c r="H34" s="34"/>
+      <c r="H34" s="24"/>
       <c r="I34" s="1" t="str">
         <f aca="false">IF($E34&lt;&gt;"",AND(config!$B$1-YEAR($E34)&gt;=Catégories!$C$16,config!$B$1-YEAR($E34)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3509,7 +3445,7 @@
       <c r="E35" s="22"/>
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
-      <c r="H35" s="34"/>
+      <c r="H35" s="24"/>
       <c r="I35" s="1" t="str">
         <f aca="false">IF($E35&lt;&gt;"",AND(config!$B$1-YEAR($E35)&gt;=Catégories!$C$16,config!$B$1-YEAR($E35)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3526,7 +3462,7 @@
       <c r="E36" s="22"/>
       <c r="F36" s="23"/>
       <c r="G36" s="23"/>
-      <c r="H36" s="34"/>
+      <c r="H36" s="24"/>
       <c r="I36" s="1" t="str">
         <f aca="false">IF($E36&lt;&gt;"",AND(config!$B$1-YEAR($E36)&gt;=Catégories!$C$16,config!$B$1-YEAR($E36)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3543,7 +3479,7 @@
       <c r="E37" s="22"/>
       <c r="F37" s="23"/>
       <c r="G37" s="23"/>
-      <c r="H37" s="34"/>
+      <c r="H37" s="24"/>
       <c r="I37" s="1" t="str">
         <f aca="false">IF($E37&lt;&gt;"",AND(config!$B$1-YEAR($E37)&gt;=Catégories!$C$16,config!$B$1-YEAR($E37)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3560,7 +3496,7 @@
       <c r="E38" s="22"/>
       <c r="F38" s="23"/>
       <c r="G38" s="23"/>
-      <c r="H38" s="34"/>
+      <c r="H38" s="24"/>
       <c r="I38" s="1" t="str">
         <f aca="false">IF($E38&lt;&gt;"",AND(config!$B$1-YEAR($E38)&gt;=Catégories!$C$16,config!$B$1-YEAR($E38)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3577,7 +3513,7 @@
       <c r="E39" s="22"/>
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
-      <c r="H39" s="34"/>
+      <c r="H39" s="24"/>
       <c r="I39" s="1" t="str">
         <f aca="false">IF($E39&lt;&gt;"",AND(config!$B$1-YEAR($E39)&gt;=Catégories!$C$16,config!$B$1-YEAR($E39)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3594,7 +3530,7 @@
       <c r="E40" s="22"/>
       <c r="F40" s="23"/>
       <c r="G40" s="23"/>
-      <c r="H40" s="34"/>
+      <c r="H40" s="24"/>
       <c r="I40" s="1" t="str">
         <f aca="false">IF($E40&lt;&gt;"",AND(config!$B$1-YEAR($E40)&gt;=Catégories!$C$16,config!$B$1-YEAR($E40)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3611,7 +3547,7 @@
       <c r="E41" s="22"/>
       <c r="F41" s="23"/>
       <c r="G41" s="23"/>
-      <c r="H41" s="34"/>
+      <c r="H41" s="24"/>
       <c r="I41" s="1" t="str">
         <f aca="false">IF($E41&lt;&gt;"",AND(config!$B$1-YEAR($E41)&gt;=Catégories!$C$16,config!$B$1-YEAR($E41)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3628,7 +3564,7 @@
       <c r="E42" s="22"/>
       <c r="F42" s="23"/>
       <c r="G42" s="23"/>
-      <c r="H42" s="34"/>
+      <c r="H42" s="24"/>
       <c r="I42" s="1" t="str">
         <f aca="false">IF($E42&lt;&gt;"",AND(config!$B$1-YEAR($E42)&gt;=Catégories!$C$16,config!$B$1-YEAR($E42)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3645,7 +3581,7 @@
       <c r="E43" s="22"/>
       <c r="F43" s="23"/>
       <c r="G43" s="23"/>
-      <c r="H43" s="34"/>
+      <c r="H43" s="24"/>
       <c r="I43" s="1" t="str">
         <f aca="false">IF($E43&lt;&gt;"",AND(config!$B$1-YEAR($E43)&gt;=Catégories!$C$16,config!$B$1-YEAR($E43)&lt;Catégories!$D$16),"")</f>
         <v/>
@@ -3756,7 +3692,7 @@
       <formula>$I5=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
+  <dataValidations count="11">
     <dataValidation allowBlank="true" errorStyle="stop" operator="notBetween" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E5:E44" type="date">
       <formula1>0</formula1>
       <formula2>18627</formula2>
@@ -3765,15 +3701,39 @@
       <formula1>100000</formula1>
       <formula2>999999</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F5:F44" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F5:F8 F11:F14" type="list">
       <formula1>Ceinture!$B$3:$B$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5 H11:H14" type="list">
       <formula1>Catégories!$N$3:$N$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6:H44" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F17:F44" type="list">
+      <formula1>Ceinture!$B$3:$B$8</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H17:H44" type="list">
+      <formula1>Catégories!$P$3:$P$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F15:F16" type="list">
+      <formula1>Ceinture!$B$3:$B$8</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H15:H16" type="list">
+      <formula1>Catégories!$P$3:$P$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F9:F10" type="list">
+      <formula1>Ceinture!$B$3:$B$8</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6:H9" type="list">
+      <formula1>Catégories!$P$3:$P$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H10" type="list">
       <formula1>Catégories!$P$3:$P$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3795,8 +3755,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3828,7 +3788,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="10" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -4713,8 +4673,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4746,7 +4706,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -4801,27 +4761,15 @@
       <c r="B5" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="22" t="n">
-        <v>29221</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="23" t="n">
-        <v>800007</v>
-      </c>
-      <c r="H5" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="32" t="b">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="1" t="str">
         <f aca="false">IF($E5&lt;&gt;"",AND(config!$B$1-YEAR($E5)&gt;=Catégories!$C$18,config!$B$1-YEAR($E5)&lt;Catégories!$D$18),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="J5" s="18"/>
       <c r="K5" s="19"/>
@@ -5608,7 +5556,7 @@
       <formula>$I5=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation allowBlank="true" errorStyle="stop" operator="notBetween" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E5:E44" type="date">
       <formula1>0</formula1>
       <formula2>18627</formula2>
@@ -5621,11 +5569,7 @@
       <formula1>Ceinture!$B$3:$B$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5" type="list">
-      <formula1>Catégories!$P$3:$P$9</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6:H44" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5:H44" type="list">
       <formula1>Catégories!$R$3:$R$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5647,8 +5591,8 @@
   </sheetPr>
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5678,7 +5622,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="10" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -6510,8 +6454,8 @@
   </sheetPr>
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6541,7 +6485,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="10" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -6591,24 +6535,14 @@
       <c r="B5" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="22" t="n">
-        <v>37987</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="23" t="n">
-        <v>800006</v>
-      </c>
-      <c r="H5" s="32" t="b">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="1" t="str">
         <f aca="false">IF($E5&lt;&gt;"",AND(config!$B$1-YEAR($E5)&gt;=Catégories!$C$20,config!$B$1-YEAR($E5)&lt;Catégories!$D$20),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="19"/>
@@ -7347,13 +7281,8 @@
   <mergeCells count="1">
     <mergeCell ref="C2:G2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C6:G44">
+  <conditionalFormatting sqref="C5:G44">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$H6=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:G5">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$H5=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7388,7 +7317,7 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -7396,7 +7325,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>11</v>
@@ -7412,7 +7341,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7420,7 +7349,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7428,7 +7357,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7436,7 +7365,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7444,7 +7373,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7452,7 +7381,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7460,7 +7389,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7468,7 +7397,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7476,7 +7405,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7484,7 +7413,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7492,7 +7421,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7500,7 +7429,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7516,7 +7445,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7524,7 +7453,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7532,7 +7461,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7540,7 +7469,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7548,7 +7477,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7556,7 +7485,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7564,7 +7493,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7572,7 +7501,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -7593,7 +7522,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -7601,7 +7530,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>11</v>
@@ -7620,7 +7549,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -7641,7 +7570,7 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -7649,7 +7578,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>11</v>
@@ -7660,7 +7589,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7668,7 +7597,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7676,7 +7605,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7684,7 +7613,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7729,7 +7658,7 @@
   </sheetPr>
   <dimension ref="A2:T20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -7740,61 +7669,61 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7811,49 +7740,49 @@
         <v>9</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7861,7 +7790,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>8</v>
@@ -7870,43 +7799,43 @@
         <v>9</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>104</v>
-      </c>
       <c r="J4" s="9" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7923,43 +7852,43 @@
         <v>11</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="K5" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>108</v>
-      </c>
       <c r="M5" s="9" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7967,7 +7896,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>9</v>
@@ -7976,43 +7905,43 @@
         <v>11</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>124</v>
+        <v>41</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>124</v>
+        <v>41</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>124</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8029,43 +7958,43 @@
         <v>13</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8073,7 +8002,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C8" s="9" t="n">
         <v>11</v>
@@ -8082,43 +8011,43 @@
         <v>13</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>28</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>124</v>
+        <v>41</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8135,31 +8064,31 @@
         <v>15</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8167,7 +8096,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C10" s="9" t="n">
         <v>13</v>
@@ -8176,22 +8105,22 @@
         <v>15</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8208,10 +8137,10 @@
         <v>18</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8219,7 +8148,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C12" s="9" t="n">
         <v>15</v>
@@ -8228,7 +8157,7 @@
         <v>18</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8245,7 +8174,7 @@
         <v>21</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8253,7 +8182,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C14" s="9" t="n">
         <v>18</v>
@@ -8262,7 +8191,7 @@
         <v>21</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8279,7 +8208,7 @@
         <v>99</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8287,7 +8216,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C16" s="9" t="n">
         <v>21</v>
@@ -8296,7 +8225,7 @@
         <v>99</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8313,7 +8242,7 @@
         <v>99</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8321,7 +8250,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C18" s="9" t="n">
         <v>30</v>
@@ -8330,7 +8259,7 @@
         <v>99</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8347,7 +8276,7 @@
         <v>99</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8355,7 +8284,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C20" s="9" t="n">
         <v>21</v>
@@ -8364,7 +8293,7 @@
         <v>99</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -8385,8 +8314,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8475,15 +8404,13 @@
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
-      <c r="E5" s="15" t="n">
-        <v>41255</v>
-      </c>
+      <c r="E5" s="15"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="18" t="n">
+      <c r="I5" s="18" t="str">
         <f aca="false">IF($E5&lt;&gt;"",AND(config!$B$1-YEAR($E5)&gt;=Catégories!$C$7,config!$B$1-YEAR($E5)&lt;Catégories!$D$7),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="J5" s="18"/>
       <c r="K5" s="19"/>
@@ -9305,7 +9232,7 @@
   </sheetPr>
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -9313,7 +9240,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B1" s="9" t="n">
         <v>2025</v>
@@ -9321,17 +9248,17 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B2" s="36" t="n">
+        <v>145</v>
+      </c>
+      <c r="B2" s="38" t="n">
         <v>45726</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="36" t="n">
+        <v>146</v>
+      </c>
+      <c r="B3" s="38" t="n">
         <v>45719</v>
       </c>
     </row>
@@ -9367,15 +9294,15 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
@@ -9457,7 +9384,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="9"/>
-      <c r="O13" s="38"/>
+      <c r="O13" s="40"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="9"/>
@@ -9498,8 +9425,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10416,8 +10343,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11334,8 +11261,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12252,8 +12179,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12345,7 +12272,7 @@
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="1" t="str">
         <f aca="false">IF($E5&lt;&gt;"",AND(config!$B$1-YEAR($E5)&gt;=Catégories!$C$11,config!$B$1-YEAR($E5)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12365,7 +12292,7 @@
       <c r="E6" s="22"/>
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
-      <c r="H6" s="24"/>
+      <c r="H6" s="31"/>
       <c r="I6" s="1" t="str">
         <f aca="false">IF($E6&lt;&gt;"",AND(config!$B$1-YEAR($E6)&gt;=Catégories!$C$11,config!$B$1-YEAR($E6)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12382,7 +12309,7 @@
       <c r="E7" s="22"/>
       <c r="F7" s="23"/>
       <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
+      <c r="H7" s="31"/>
       <c r="I7" s="1" t="str">
         <f aca="false">IF($E7&lt;&gt;"",AND(config!$B$1-YEAR($E7)&gt;=Catégories!$C$11,config!$B$1-YEAR($E7)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12399,7 +12326,7 @@
       <c r="E8" s="22"/>
       <c r="F8" s="23"/>
       <c r="G8" s="23"/>
-      <c r="H8" s="24"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="1" t="str">
         <f aca="false">IF($E8&lt;&gt;"",AND(config!$B$1-YEAR($E8)&gt;=Catégories!$C$11,config!$B$1-YEAR($E8)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12416,7 +12343,7 @@
       <c r="E9" s="22"/>
       <c r="F9" s="23"/>
       <c r="G9" s="23"/>
-      <c r="H9" s="24"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="1" t="str">
         <f aca="false">IF($E9&lt;&gt;"",AND(config!$B$1-YEAR($E9)&gt;=Catégories!$C$11,config!$B$1-YEAR($E9)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12433,7 +12360,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="1" t="str">
         <f aca="false">IF($E10&lt;&gt;"",AND(config!$B$1-YEAR($E10)&gt;=Catégories!$C$11,config!$B$1-YEAR($E10)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12450,7 +12377,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
+      <c r="H11" s="31"/>
       <c r="I11" s="1" t="str">
         <f aca="false">IF($E11&lt;&gt;"",AND(config!$B$1-YEAR($E11)&gt;=Catégories!$C$11,config!$B$1-YEAR($E11)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12470,7 +12397,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
+      <c r="H12" s="31"/>
       <c r="I12" s="1" t="str">
         <f aca="false">IF($E12&lt;&gt;"",AND(config!$B$1-YEAR($E12)&gt;=Catégories!$C$11,config!$B$1-YEAR($E12)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12490,7 +12417,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
+      <c r="H13" s="31"/>
       <c r="I13" s="1" t="str">
         <f aca="false">IF($E13&lt;&gt;"",AND(config!$B$1-YEAR($E13)&gt;=Catégories!$C$11,config!$B$1-YEAR($E13)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12510,7 +12437,7 @@
       <c r="E14" s="22"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
+      <c r="H14" s="31"/>
       <c r="I14" s="1" t="str">
         <f aca="false">IF($E14&lt;&gt;"",AND(config!$B$1-YEAR($E14)&gt;=Catégories!$C$11,config!$B$1-YEAR($E14)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12530,7 +12457,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="31"/>
       <c r="I15" s="1" t="str">
         <f aca="false">IF($E15&lt;&gt;"",AND(config!$B$1-YEAR($E15)&gt;=Catégories!$C$11,config!$B$1-YEAR($E15)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12550,7 +12477,7 @@
       <c r="E16" s="22"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="24"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="1" t="str">
         <f aca="false">IF($E16&lt;&gt;"",AND(config!$B$1-YEAR($E16)&gt;=Catégories!$C$11,config!$B$1-YEAR($E16)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12570,7 +12497,7 @@
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
-      <c r="H17" s="24"/>
+      <c r="H17" s="31"/>
       <c r="I17" s="1" t="str">
         <f aca="false">IF($E17&lt;&gt;"",AND(config!$B$1-YEAR($E17)&gt;=Catégories!$C$11,config!$B$1-YEAR($E17)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12590,7 +12517,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
-      <c r="H18" s="24"/>
+      <c r="H18" s="31"/>
       <c r="I18" s="1" t="str">
         <f aca="false">IF($E18&lt;&gt;"",AND(config!$B$1-YEAR($E18)&gt;=Catégories!$C$11,config!$B$1-YEAR($E18)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12610,7 +12537,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="23"/>
       <c r="G19" s="23"/>
-      <c r="H19" s="24"/>
+      <c r="H19" s="31"/>
       <c r="I19" s="1" t="str">
         <f aca="false">IF($E19&lt;&gt;"",AND(config!$B$1-YEAR($E19)&gt;=Catégories!$C$11,config!$B$1-YEAR($E19)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12630,7 +12557,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="23"/>
       <c r="G20" s="23"/>
-      <c r="H20" s="24"/>
+      <c r="H20" s="31"/>
       <c r="I20" s="1" t="str">
         <f aca="false">IF($E20&lt;&gt;"",AND(config!$B$1-YEAR($E20)&gt;=Catégories!$C$11,config!$B$1-YEAR($E20)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12650,7 +12577,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="23"/>
       <c r="G21" s="23"/>
-      <c r="H21" s="24"/>
+      <c r="H21" s="31"/>
       <c r="I21" s="1" t="str">
         <f aca="false">IF($E21&lt;&gt;"",AND(config!$B$1-YEAR($E21)&gt;=Catégories!$C$11,config!$B$1-YEAR($E21)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12667,7 +12594,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="23"/>
       <c r="G22" s="23"/>
-      <c r="H22" s="24"/>
+      <c r="H22" s="31"/>
       <c r="I22" s="1" t="str">
         <f aca="false">IF($E22&lt;&gt;"",AND(config!$B$1-YEAR($E22)&gt;=Catégories!$C$11,config!$B$1-YEAR($E22)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12684,7 +12611,7 @@
       <c r="E23" s="22"/>
       <c r="F23" s="23"/>
       <c r="G23" s="23"/>
-      <c r="H23" s="24"/>
+      <c r="H23" s="31"/>
       <c r="I23" s="1" t="str">
         <f aca="false">IF($E23&lt;&gt;"",AND(config!$B$1-YEAR($E23)&gt;=Catégories!$C$11,config!$B$1-YEAR($E23)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12701,7 +12628,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="23"/>
       <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="1" t="str">
         <f aca="false">IF($E24&lt;&gt;"",AND(config!$B$1-YEAR($E24)&gt;=Catégories!$C$11,config!$B$1-YEAR($E24)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12718,7 +12645,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="23"/>
       <c r="G25" s="23"/>
-      <c r="H25" s="24"/>
+      <c r="H25" s="31"/>
       <c r="I25" s="1" t="str">
         <f aca="false">IF($E25&lt;&gt;"",AND(config!$B$1-YEAR($E25)&gt;=Catégories!$C$11,config!$B$1-YEAR($E25)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12735,7 +12662,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="23"/>
       <c r="G26" s="23"/>
-      <c r="H26" s="24"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="1" t="str">
         <f aca="false">IF($E26&lt;&gt;"",AND(config!$B$1-YEAR($E26)&gt;=Catégories!$C$11,config!$B$1-YEAR($E26)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12752,7 +12679,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
-      <c r="H27" s="24"/>
+      <c r="H27" s="31"/>
       <c r="I27" s="1" t="str">
         <f aca="false">IF($E27&lt;&gt;"",AND(config!$B$1-YEAR($E27)&gt;=Catégories!$C$11,config!$B$1-YEAR($E27)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12769,7 +12696,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="23"/>
       <c r="G28" s="23"/>
-      <c r="H28" s="24"/>
+      <c r="H28" s="31"/>
       <c r="I28" s="1" t="str">
         <f aca="false">IF($E28&lt;&gt;"",AND(config!$B$1-YEAR($E28)&gt;=Catégories!$C$11,config!$B$1-YEAR($E28)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12786,7 +12713,7 @@
       <c r="E29" s="22"/>
       <c r="F29" s="23"/>
       <c r="G29" s="23"/>
-      <c r="H29" s="24"/>
+      <c r="H29" s="31"/>
       <c r="I29" s="1" t="str">
         <f aca="false">IF($E29&lt;&gt;"",AND(config!$B$1-YEAR($E29)&gt;=Catégories!$C$11,config!$B$1-YEAR($E29)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12803,7 +12730,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="23"/>
       <c r="G30" s="23"/>
-      <c r="H30" s="24"/>
+      <c r="H30" s="31"/>
       <c r="I30" s="1" t="str">
         <f aca="false">IF($E30&lt;&gt;"",AND(config!$B$1-YEAR($E30)&gt;=Catégories!$C$11,config!$B$1-YEAR($E30)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12820,7 +12747,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="23"/>
       <c r="G31" s="23"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="31"/>
       <c r="I31" s="1" t="str">
         <f aca="false">IF($E31&lt;&gt;"",AND(config!$B$1-YEAR($E31)&gt;=Catégories!$C$11,config!$B$1-YEAR($E31)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12837,7 +12764,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
-      <c r="H32" s="24"/>
+      <c r="H32" s="31"/>
       <c r="I32" s="1" t="str">
         <f aca="false">IF($E32&lt;&gt;"",AND(config!$B$1-YEAR($E32)&gt;=Catégories!$C$11,config!$B$1-YEAR($E32)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12854,7 +12781,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>
-      <c r="H33" s="24"/>
+      <c r="H33" s="31"/>
       <c r="I33" s="1" t="str">
         <f aca="false">IF($E33&lt;&gt;"",AND(config!$B$1-YEAR($E33)&gt;=Catégories!$C$11,config!$B$1-YEAR($E33)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12871,7 +12798,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
-      <c r="H34" s="24"/>
+      <c r="H34" s="31"/>
       <c r="I34" s="1" t="str">
         <f aca="false">IF($E34&lt;&gt;"",AND(config!$B$1-YEAR($E34)&gt;=Catégories!$C$11,config!$B$1-YEAR($E34)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12888,7 +12815,7 @@
       <c r="E35" s="22"/>
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
-      <c r="H35" s="24"/>
+      <c r="H35" s="31"/>
       <c r="I35" s="1" t="str">
         <f aca="false">IF($E35&lt;&gt;"",AND(config!$B$1-YEAR($E35)&gt;=Catégories!$C$11,config!$B$1-YEAR($E35)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12905,7 +12832,7 @@
       <c r="E36" s="22"/>
       <c r="F36" s="23"/>
       <c r="G36" s="23"/>
-      <c r="H36" s="24"/>
+      <c r="H36" s="31"/>
       <c r="I36" s="1" t="str">
         <f aca="false">IF($E36&lt;&gt;"",AND(config!$B$1-YEAR($E36)&gt;=Catégories!$C$11,config!$B$1-YEAR($E36)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12922,7 +12849,7 @@
       <c r="E37" s="22"/>
       <c r="F37" s="23"/>
       <c r="G37" s="23"/>
-      <c r="H37" s="24"/>
+      <c r="H37" s="31"/>
       <c r="I37" s="1" t="str">
         <f aca="false">IF($E37&lt;&gt;"",AND(config!$B$1-YEAR($E37)&gt;=Catégories!$C$11,config!$B$1-YEAR($E37)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12939,7 +12866,7 @@
       <c r="E38" s="22"/>
       <c r="F38" s="23"/>
       <c r="G38" s="23"/>
-      <c r="H38" s="24"/>
+      <c r="H38" s="31"/>
       <c r="I38" s="1" t="str">
         <f aca="false">IF($E38&lt;&gt;"",AND(config!$B$1-YEAR($E38)&gt;=Catégories!$C$11,config!$B$1-YEAR($E38)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12956,7 +12883,7 @@
       <c r="E39" s="22"/>
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
-      <c r="H39" s="24"/>
+      <c r="H39" s="31"/>
       <c r="I39" s="1" t="str">
         <f aca="false">IF($E39&lt;&gt;"",AND(config!$B$1-YEAR($E39)&gt;=Catégories!$C$11,config!$B$1-YEAR($E39)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12973,7 +12900,7 @@
       <c r="E40" s="22"/>
       <c r="F40" s="23"/>
       <c r="G40" s="23"/>
-      <c r="H40" s="24"/>
+      <c r="H40" s="31"/>
       <c r="I40" s="1" t="str">
         <f aca="false">IF($E40&lt;&gt;"",AND(config!$B$1-YEAR($E40)&gt;=Catégories!$C$11,config!$B$1-YEAR($E40)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -12990,7 +12917,7 @@
       <c r="E41" s="22"/>
       <c r="F41" s="23"/>
       <c r="G41" s="23"/>
-      <c r="H41" s="24"/>
+      <c r="H41" s="31"/>
       <c r="I41" s="1" t="str">
         <f aca="false">IF($E41&lt;&gt;"",AND(config!$B$1-YEAR($E41)&gt;=Catégories!$C$11,config!$B$1-YEAR($E41)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -13007,7 +12934,7 @@
       <c r="E42" s="22"/>
       <c r="F42" s="23"/>
       <c r="G42" s="23"/>
-      <c r="H42" s="24"/>
+      <c r="H42" s="31"/>
       <c r="I42" s="1" t="str">
         <f aca="false">IF($E42&lt;&gt;"",AND(config!$B$1-YEAR($E42)&gt;=Catégories!$C$11,config!$B$1-YEAR($E42)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -13024,7 +12951,7 @@
       <c r="E43" s="22"/>
       <c r="F43" s="23"/>
       <c r="G43" s="23"/>
-      <c r="H43" s="24"/>
+      <c r="H43" s="31"/>
       <c r="I43" s="1" t="str">
         <f aca="false">IF($E43&lt;&gt;"",AND(config!$B$1-YEAR($E43)&gt;=Catégories!$C$11,config!$B$1-YEAR($E43)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -13041,7 +12968,7 @@
       <c r="E44" s="27"/>
       <c r="F44" s="28"/>
       <c r="G44" s="28"/>
-      <c r="H44" s="29"/>
+      <c r="H44" s="32"/>
       <c r="I44" s="1" t="str">
         <f aca="false">IF($E44&lt;&gt;"",AND(config!$B$1-YEAR($E44)&gt;=Catégories!$C$11,config!$B$1-YEAR($E44)&lt;Catégories!$D$11),"")</f>
         <v/>
@@ -13170,8 +13097,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14088,8 +14015,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15006,8 +14933,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15103,16 +15030,16 @@
       <c r="E5" s="15" t="n">
         <v>38718</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="33" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="16" t="n">
         <v>800001</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="32" t="b">
+      <c r="I5" s="35" t="b">
         <f aca="false">IF($E5&lt;&gt;"",AND(config!$B$1-YEAR($E5)&gt;=Catégories!$C$14,config!$B$1-YEAR($E5)&lt;Catégories!$D$14),"")</f>
         <v>1</v>
       </c>
@@ -15135,16 +15062,16 @@
       <c r="E6" s="22" t="n">
         <v>38718</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="36" t="s">
         <v>31</v>
       </c>
       <c r="G6" s="23" t="n">
         <v>800002</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="32" t="b">
+      <c r="I6" s="35" t="b">
         <f aca="false">IF($E6&lt;&gt;"",AND(config!$B$1-YEAR($E6)&gt;=Catégories!$C$14,config!$B$1-YEAR($E6)&lt;Catégories!$D$14),"")</f>
         <v>1</v>
       </c>
@@ -15164,16 +15091,16 @@
       <c r="E7" s="22" t="n">
         <v>38718</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="36" t="s">
         <v>31</v>
       </c>
       <c r="G7" s="23" t="n">
         <v>800003</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="32" t="b">
+      <c r="I7" s="35" t="b">
         <f aca="false">IF($E7&lt;&gt;"",AND(config!$B$1-YEAR($E7)&gt;=Catégories!$C$14,config!$B$1-YEAR($E7)&lt;Catégories!$D$14),"")</f>
         <v>1</v>
       </c>
@@ -15193,16 +15120,16 @@
       <c r="E8" s="22" t="n">
         <v>38718</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="36" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="23" t="n">
         <v>800004</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="32" t="b">
+      <c r="I8" s="35" t="b">
         <f aca="false">IF($E8&lt;&gt;"",AND(config!$B$1-YEAR($E8)&gt;=Catégories!$C$14,config!$B$1-YEAR($E8)&lt;Catégories!$D$14),"")</f>
         <v>1</v>
       </c>
@@ -15222,16 +15149,16 @@
       <c r="E9" s="22" t="n">
         <v>38718</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="23" t="n">
         <v>800005</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="32" t="b">
+      <c r="I9" s="35" t="b">
         <f aca="false">IF($E9&lt;&gt;"",AND(config!$B$1-YEAR($E9)&gt;=Catégories!$C$14,config!$B$1-YEAR($E9)&lt;Catégories!$D$14),"")</f>
         <v>1</v>
       </c>
@@ -15242,11 +15169,11 @@
       <c r="B10" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="33"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="34"/>
       <c r="I10" s="1" t="str">
         <f aca="false">IF($E10&lt;&gt;"",AND(config!$B$1-YEAR($E10)&gt;=Catégories!$C$14,config!$B$1-YEAR($E10)&lt;Catégories!$D$14),"")</f>
@@ -15262,9 +15189,9 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
-      <c r="F11" s="33"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="23"/>
-      <c r="H11" s="34"/>
+      <c r="H11" s="37"/>
       <c r="I11" s="1" t="str">
         <f aca="false">IF($E11&lt;&gt;"",AND(config!$B$1-YEAR($E11)&gt;=Catégories!$C$14,config!$B$1-YEAR($E11)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15282,9 +15209,9 @@
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
-      <c r="F12" s="33"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="23"/>
-      <c r="H12" s="34"/>
+      <c r="H12" s="37"/>
       <c r="I12" s="1" t="str">
         <f aca="false">IF($E12&lt;&gt;"",AND(config!$B$1-YEAR($E12)&gt;=Catégories!$C$14,config!$B$1-YEAR($E12)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15302,9 +15229,9 @@
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
-      <c r="F13" s="33"/>
+      <c r="F13" s="36"/>
       <c r="G13" s="23"/>
-      <c r="H13" s="34"/>
+      <c r="H13" s="37"/>
       <c r="I13" s="1" t="str">
         <f aca="false">IF($E13&lt;&gt;"",AND(config!$B$1-YEAR($E13)&gt;=Catégories!$C$14,config!$B$1-YEAR($E13)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15322,9 +15249,9 @@
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
-      <c r="F14" s="33"/>
+      <c r="F14" s="36"/>
       <c r="G14" s="23"/>
-      <c r="H14" s="34"/>
+      <c r="H14" s="37"/>
       <c r="I14" s="1" t="str">
         <f aca="false">IF($E14&lt;&gt;"",AND(config!$B$1-YEAR($E14)&gt;=Catégories!$C$14,config!$B$1-YEAR($E14)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15342,9 +15269,9 @@
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
-      <c r="F15" s="33"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="23"/>
-      <c r="H15" s="34"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="1" t="str">
         <f aca="false">IF($E15&lt;&gt;"",AND(config!$B$1-YEAR($E15)&gt;=Catégories!$C$14,config!$B$1-YEAR($E15)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15362,9 +15289,9 @@
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
       <c r="E16" s="22"/>
-      <c r="F16" s="33"/>
+      <c r="F16" s="36"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="34"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="1" t="str">
         <f aca="false">IF($E16&lt;&gt;"",AND(config!$B$1-YEAR($E16)&gt;=Catégories!$C$14,config!$B$1-YEAR($E16)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15382,9 +15309,9 @@
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
       <c r="E17" s="22"/>
-      <c r="F17" s="33"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="23"/>
-      <c r="H17" s="34"/>
+      <c r="H17" s="24"/>
       <c r="I17" s="1" t="str">
         <f aca="false">IF($E17&lt;&gt;"",AND(config!$B$1-YEAR($E17)&gt;=Catégories!$C$14,config!$B$1-YEAR($E17)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15402,9 +15329,9 @@
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
       <c r="E18" s="22"/>
-      <c r="F18" s="33"/>
+      <c r="F18" s="23"/>
       <c r="G18" s="23"/>
-      <c r="H18" s="34"/>
+      <c r="H18" s="24"/>
       <c r="I18" s="1" t="str">
         <f aca="false">IF($E18&lt;&gt;"",AND(config!$B$1-YEAR($E18)&gt;=Catégories!$C$14,config!$B$1-YEAR($E18)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15422,9 +15349,9 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
       <c r="E19" s="22"/>
-      <c r="F19" s="33"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="23"/>
-      <c r="H19" s="34"/>
+      <c r="H19" s="24"/>
       <c r="I19" s="1" t="str">
         <f aca="false">IF($E19&lt;&gt;"",AND(config!$B$1-YEAR($E19)&gt;=Catégories!$C$14,config!$B$1-YEAR($E19)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15442,9 +15369,9 @@
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
       <c r="E20" s="22"/>
-      <c r="F20" s="33"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="23"/>
-      <c r="H20" s="34"/>
+      <c r="H20" s="24"/>
       <c r="I20" s="1" t="str">
         <f aca="false">IF($E20&lt;&gt;"",AND(config!$B$1-YEAR($E20)&gt;=Catégories!$C$14,config!$B$1-YEAR($E20)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15462,9 +15389,9 @@
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="22"/>
-      <c r="F21" s="33"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="23"/>
-      <c r="H21" s="34"/>
+      <c r="H21" s="24"/>
       <c r="I21" s="1" t="str">
         <f aca="false">IF($E21&lt;&gt;"",AND(config!$B$1-YEAR($E21)&gt;=Catégories!$C$14,config!$B$1-YEAR($E21)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15479,9 +15406,9 @@
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
       <c r="E22" s="22"/>
-      <c r="F22" s="33"/>
+      <c r="F22" s="23"/>
       <c r="G22" s="23"/>
-      <c r="H22" s="34"/>
+      <c r="H22" s="24"/>
       <c r="I22" s="1" t="str">
         <f aca="false">IF($E22&lt;&gt;"",AND(config!$B$1-YEAR($E22)&gt;=Catégories!$C$14,config!$B$1-YEAR($E22)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15496,9 +15423,9 @@
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="22"/>
-      <c r="F23" s="33"/>
+      <c r="F23" s="23"/>
       <c r="G23" s="23"/>
-      <c r="H23" s="34"/>
+      <c r="H23" s="24"/>
       <c r="I23" s="1" t="str">
         <f aca="false">IF($E23&lt;&gt;"",AND(config!$B$1-YEAR($E23)&gt;=Catégories!$C$14,config!$B$1-YEAR($E23)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15513,9 +15440,9 @@
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="22"/>
-      <c r="F24" s="33"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="23"/>
-      <c r="H24" s="34"/>
+      <c r="H24" s="24"/>
       <c r="I24" s="1" t="str">
         <f aca="false">IF($E24&lt;&gt;"",AND(config!$B$1-YEAR($E24)&gt;=Catégories!$C$14,config!$B$1-YEAR($E24)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15530,9 +15457,9 @@
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="22"/>
-      <c r="F25" s="33"/>
+      <c r="F25" s="23"/>
       <c r="G25" s="23"/>
-      <c r="H25" s="34"/>
+      <c r="H25" s="24"/>
       <c r="I25" s="1" t="str">
         <f aca="false">IF($E25&lt;&gt;"",AND(config!$B$1-YEAR($E25)&gt;=Catégories!$C$14,config!$B$1-YEAR($E25)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15547,9 +15474,9 @@
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
       <c r="E26" s="22"/>
-      <c r="F26" s="33"/>
+      <c r="F26" s="23"/>
       <c r="G26" s="23"/>
-      <c r="H26" s="34"/>
+      <c r="H26" s="24"/>
       <c r="I26" s="1" t="str">
         <f aca="false">IF($E26&lt;&gt;"",AND(config!$B$1-YEAR($E26)&gt;=Catégories!$C$14,config!$B$1-YEAR($E26)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15564,9 +15491,9 @@
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
-      <c r="F27" s="33"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="23"/>
-      <c r="H27" s="34"/>
+      <c r="H27" s="24"/>
       <c r="I27" s="1" t="str">
         <f aca="false">IF($E27&lt;&gt;"",AND(config!$B$1-YEAR($E27)&gt;=Catégories!$C$14,config!$B$1-YEAR($E27)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15581,9 +15508,9 @@
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
-      <c r="F28" s="33"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="23"/>
-      <c r="H28" s="34"/>
+      <c r="H28" s="24"/>
       <c r="I28" s="1" t="str">
         <f aca="false">IF($E28&lt;&gt;"",AND(config!$B$1-YEAR($E28)&gt;=Catégories!$C$14,config!$B$1-YEAR($E28)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15598,9 +15525,9 @@
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
       <c r="E29" s="22"/>
-      <c r="F29" s="33"/>
+      <c r="F29" s="23"/>
       <c r="G29" s="23"/>
-      <c r="H29" s="34"/>
+      <c r="H29" s="24"/>
       <c r="I29" s="1" t="str">
         <f aca="false">IF($E29&lt;&gt;"",AND(config!$B$1-YEAR($E29)&gt;=Catégories!$C$14,config!$B$1-YEAR($E29)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15615,9 +15542,9 @@
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
-      <c r="F30" s="33"/>
+      <c r="F30" s="23"/>
       <c r="G30" s="23"/>
-      <c r="H30" s="34"/>
+      <c r="H30" s="24"/>
       <c r="I30" s="1" t="str">
         <f aca="false">IF($E30&lt;&gt;"",AND(config!$B$1-YEAR($E30)&gt;=Catégories!$C$14,config!$B$1-YEAR($E30)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15632,9 +15559,9 @@
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
       <c r="E31" s="22"/>
-      <c r="F31" s="33"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="23"/>
-      <c r="H31" s="34"/>
+      <c r="H31" s="24"/>
       <c r="I31" s="1" t="str">
         <f aca="false">IF($E31&lt;&gt;"",AND(config!$B$1-YEAR($E31)&gt;=Catégories!$C$14,config!$B$1-YEAR($E31)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15649,9 +15576,9 @@
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
       <c r="E32" s="22"/>
-      <c r="F32" s="33"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="23"/>
-      <c r="H32" s="34"/>
+      <c r="H32" s="24"/>
       <c r="I32" s="1" t="str">
         <f aca="false">IF($E32&lt;&gt;"",AND(config!$B$1-YEAR($E32)&gt;=Catégories!$C$14,config!$B$1-YEAR($E32)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15666,9 +15593,9 @@
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
       <c r="E33" s="22"/>
-      <c r="F33" s="33"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="23"/>
-      <c r="H33" s="34"/>
+      <c r="H33" s="24"/>
       <c r="I33" s="1" t="str">
         <f aca="false">IF($E33&lt;&gt;"",AND(config!$B$1-YEAR($E33)&gt;=Catégories!$C$14,config!$B$1-YEAR($E33)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15683,9 +15610,9 @@
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
       <c r="E34" s="22"/>
-      <c r="F34" s="33"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="23"/>
-      <c r="H34" s="34"/>
+      <c r="H34" s="24"/>
       <c r="I34" s="1" t="str">
         <f aca="false">IF($E34&lt;&gt;"",AND(config!$B$1-YEAR($E34)&gt;=Catégories!$C$14,config!$B$1-YEAR($E34)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15700,9 +15627,9 @@
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
-      <c r="F35" s="33"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="23"/>
-      <c r="H35" s="34"/>
+      <c r="H35" s="24"/>
       <c r="I35" s="1" t="str">
         <f aca="false">IF($E35&lt;&gt;"",AND(config!$B$1-YEAR($E35)&gt;=Catégories!$C$14,config!$B$1-YEAR($E35)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15717,9 +15644,9 @@
       <c r="C36" s="21"/>
       <c r="D36" s="21"/>
       <c r="E36" s="22"/>
-      <c r="F36" s="33"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="23"/>
-      <c r="H36" s="34"/>
+      <c r="H36" s="24"/>
       <c r="I36" s="1" t="str">
         <f aca="false">IF($E36&lt;&gt;"",AND(config!$B$1-YEAR($E36)&gt;=Catégories!$C$14,config!$B$1-YEAR($E36)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15734,9 +15661,9 @@
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
       <c r="E37" s="22"/>
-      <c r="F37" s="33"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="23"/>
-      <c r="H37" s="34"/>
+      <c r="H37" s="24"/>
       <c r="I37" s="1" t="str">
         <f aca="false">IF($E37&lt;&gt;"",AND(config!$B$1-YEAR($E37)&gt;=Catégories!$C$14,config!$B$1-YEAR($E37)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15751,9 +15678,9 @@
       <c r="C38" s="21"/>
       <c r="D38" s="21"/>
       <c r="E38" s="22"/>
-      <c r="F38" s="33"/>
+      <c r="F38" s="23"/>
       <c r="G38" s="23"/>
-      <c r="H38" s="34"/>
+      <c r="H38" s="24"/>
       <c r="I38" s="1" t="str">
         <f aca="false">IF($E38&lt;&gt;"",AND(config!$B$1-YEAR($E38)&gt;=Catégories!$C$14,config!$B$1-YEAR($E38)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15768,9 +15695,9 @@
       <c r="C39" s="21"/>
       <c r="D39" s="21"/>
       <c r="E39" s="22"/>
-      <c r="F39" s="33"/>
+      <c r="F39" s="23"/>
       <c r="G39" s="23"/>
-      <c r="H39" s="34"/>
+      <c r="H39" s="24"/>
       <c r="I39" s="1" t="str">
         <f aca="false">IF($E39&lt;&gt;"",AND(config!$B$1-YEAR($E39)&gt;=Catégories!$C$14,config!$B$1-YEAR($E39)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15785,9 +15712,9 @@
       <c r="C40" s="21"/>
       <c r="D40" s="21"/>
       <c r="E40" s="22"/>
-      <c r="F40" s="33"/>
+      <c r="F40" s="23"/>
       <c r="G40" s="23"/>
-      <c r="H40" s="34"/>
+      <c r="H40" s="24"/>
       <c r="I40" s="1" t="str">
         <f aca="false">IF($E40&lt;&gt;"",AND(config!$B$1-YEAR($E40)&gt;=Catégories!$C$14,config!$B$1-YEAR($E40)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15802,9 +15729,9 @@
       <c r="C41" s="21"/>
       <c r="D41" s="21"/>
       <c r="E41" s="22"/>
-      <c r="F41" s="33"/>
+      <c r="F41" s="23"/>
       <c r="G41" s="23"/>
-      <c r="H41" s="34"/>
+      <c r="H41" s="24"/>
       <c r="I41" s="1" t="str">
         <f aca="false">IF($E41&lt;&gt;"",AND(config!$B$1-YEAR($E41)&gt;=Catégories!$C$14,config!$B$1-YEAR($E41)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15819,9 +15746,9 @@
       <c r="C42" s="21"/>
       <c r="D42" s="21"/>
       <c r="E42" s="22"/>
-      <c r="F42" s="33"/>
+      <c r="F42" s="23"/>
       <c r="G42" s="23"/>
-      <c r="H42" s="34"/>
+      <c r="H42" s="24"/>
       <c r="I42" s="1" t="str">
         <f aca="false">IF($E42&lt;&gt;"",AND(config!$B$1-YEAR($E42)&gt;=Catégories!$C$14,config!$B$1-YEAR($E42)&lt;Catégories!$D$14),"")</f>
         <v/>
@@ -15836,9 +15763,9 @@
       <c r="C43" s="21"/>
       <c r="D43" s="21"/>
       <c r="E43" s="22"/>
-      <c r="F43" s="33"/>
+      <c r="F43" s="23"/>
       <c r="G43" s="23"/>
-      <c r="H43" s="34"/>
+      <c r="H43" s="24"/>
       <c r="I43" s="1" t="str">
         <f aca="false">IF($E43&lt;&gt;"",AND(config!$B$1-YEAR($E43)&gt;=Catégories!$C$14,config!$B$1-YEAR($E43)&lt;Catégories!$D$14),"")</f>
         <v/>

</xml_diff>